<commit_message>
Organiza el excel de resultados de resampling
</commit_message>
<xml_diff>
--- a/data/resultados_resampling.xlsx
+++ b/data/resultados_resampling.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pasal\Google Drive\EAFIT\Ciencia de Datos y Analitica\02 Segundo Semestre\Proyecto Integrador\Proyecto-Integrador-2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80567695-7F6B-400B-BAA6-76877B92D766}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90FC7F71-2FBE-4F66-92B7-88A37F7989AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0A39EE4B-5006-4E29-BC75-38928D5F2EAA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{0A39EE4B-5006-4E29-BC75-38928D5F2EAA}"/>
   </bookViews>
   <sheets>
     <sheet name="NN" sheetId="1" r:id="rId1"/>
-    <sheet name="RF" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja1" sheetId="3" r:id="rId2"/>
+    <sheet name="RF" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">NN!$G$3:$H$67</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">RF!$G$3:$H$66</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">RF!$G$3:$H$66</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="21">
   <si>
     <t xml:space="preserve"> Inica TOMEKLINKS</t>
   </si>
@@ -96,13 +97,19 @@
   <si>
     <t xml:space="preserve"> SMOTEENN</t>
   </si>
+  <si>
+    <t>Proporcion</t>
+  </si>
+  <si>
+    <t>Tecnica</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -157,13 +164,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -481,27 +492,27 @@
   <sheetPr filterMode="1"/>
   <dimension ref="G1:M67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6:M62"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H77" sqref="H77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="7" max="7" width="35" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="62.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="62.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="7:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="7:13" x14ac:dyDescent="0.3">
       <c r="H1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="7:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="7:13" x14ac:dyDescent="0.3">
       <c r="H2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="7:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="7:13" x14ac:dyDescent="0.3">
       <c r="H3" s="1" t="s">
         <v>3</v>
       </c>
@@ -521,7 +532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="H4" t="s">
         <v>4</v>
       </c>
@@ -541,7 +552,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G5" t="s">
         <v>4</v>
       </c>
@@ -564,7 +575,7 @@
         <v>0.78027937259757996</v>
       </c>
     </row>
-    <row r="6" spans="7:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="7:13" x14ac:dyDescent="0.3">
       <c r="G6" t="s">
         <v>4</v>
       </c>
@@ -587,7 +598,7 @@
         <v>5.7933169700369401E-2</v>
       </c>
     </row>
-    <row r="7" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G7" t="s">
         <v>4</v>
       </c>
@@ -610,7 +621,7 @@
         <v>8.01990928430939E-2</v>
       </c>
     </row>
-    <row r="8" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G8" t="s">
         <v>4</v>
       </c>
@@ -633,7 +644,7 @@
         <v>0.70804307895642904</v>
       </c>
     </row>
-    <row r="9" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G9" t="s">
         <v>4</v>
       </c>
@@ -656,7 +667,7 @@
         <v>4.2465462274176399E-2</v>
       </c>
     </row>
-    <row r="10" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G10" t="s">
         <v>4</v>
       </c>
@@ -679,12 +690,12 @@
         <v>0.71974063400576305</v>
       </c>
     </row>
-    <row r="11" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="H11" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="H12" t="s">
         <v>12</v>
       </c>
@@ -704,7 +715,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G13" t="s">
         <v>12</v>
       </c>
@@ -727,7 +738,7 @@
         <v>0.78321298163615205</v>
       </c>
     </row>
-    <row r="14" spans="7:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="7:13" x14ac:dyDescent="0.3">
       <c r="G14" t="s">
         <v>12</v>
       </c>
@@ -750,7 +761,7 @@
         <v>5.9261662580175199E-2</v>
       </c>
     </row>
-    <row r="15" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G15" t="s">
         <v>12</v>
       </c>
@@ -773,7 +784,7 @@
         <v>8.2497305364397602E-2</v>
       </c>
     </row>
-    <row r="16" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G16" t="s">
         <v>12</v>
       </c>
@@ -796,7 +807,7 @@
         <v>0.71190660657278604</v>
       </c>
     </row>
-    <row r="17" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G17" t="s">
         <v>12</v>
       </c>
@@ -819,7 +830,7 @@
         <v>4.3767044954693399E-2</v>
       </c>
     </row>
-    <row r="18" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G18" t="s">
         <v>12</v>
       </c>
@@ -842,12 +853,12 @@
         <v>0.71685878962535998</v>
       </c>
     </row>
-    <row r="19" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="H19" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="H20" t="s">
         <v>13</v>
       </c>
@@ -867,7 +878,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G21" t="s">
         <v>13</v>
       </c>
@@ -890,7 +901,7 @@
         <v>0.77926287204464095</v>
       </c>
     </row>
-    <row r="22" spans="7:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="7:13" x14ac:dyDescent="0.3">
       <c r="G22" t="s">
         <v>13</v>
       </c>
@@ -913,7 +924,7 @@
         <v>5.8675491365870198E-2</v>
       </c>
     </row>
-    <row r="23" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G23" t="s">
         <v>13</v>
       </c>
@@ -936,7 +947,7 @@
         <v>8.1695793962705904E-2</v>
       </c>
     </row>
-    <row r="24" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G24" t="s">
         <v>13</v>
       </c>
@@ -959,7 +970,7 @@
         <v>0.70667611321499801</v>
       </c>
     </row>
-    <row r="25" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G25" t="s">
         <v>13</v>
       </c>
@@ -982,7 +993,7 @@
         <v>4.3364403018197897E-2</v>
       </c>
     </row>
-    <row r="26" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G26" t="s">
         <v>13</v>
       </c>
@@ -1005,12 +1016,12 @@
         <v>0.70389048991354397</v>
       </c>
     </row>
-    <row r="27" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="H27" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="H28" t="s">
         <v>14</v>
       </c>
@@ -1030,7 +1041,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G29" t="s">
         <v>14</v>
       </c>
@@ -1053,7 +1064,7 @@
         <v>0.70204043268494698</v>
       </c>
     </row>
-    <row r="30" spans="7:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="7:13" x14ac:dyDescent="0.3">
       <c r="G30" t="s">
         <v>14</v>
       </c>
@@ -1076,7 +1087,7 @@
         <v>3.6736872561912902E-2</v>
       </c>
     </row>
-    <row r="31" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G31" t="s">
         <v>14</v>
       </c>
@@ -1099,7 +1110,7 @@
         <v>4.8512353044736903E-2</v>
       </c>
     </row>
-    <row r="32" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G32" t="s">
         <v>14</v>
       </c>
@@ -1122,7 +1133,7 @@
         <v>0.61983875765441898</v>
       </c>
     </row>
-    <row r="33" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G33" t="s">
         <v>14</v>
       </c>
@@ -1145,7 +1156,7 @@
         <v>2.4933142983532001E-2</v>
       </c>
     </row>
-    <row r="34" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G34" t="s">
         <v>14</v>
       </c>
@@ -1168,12 +1179,12 @@
         <v>0.89337175792507195</v>
       </c>
     </row>
-    <row r="35" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="H35" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="H36" t="s">
         <v>15</v>
       </c>
@@ -1193,7 +1204,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G37" t="s">
         <v>15</v>
       </c>
@@ -1216,7 +1227,7 @@
         <v>0.77514059883298903</v>
       </c>
     </row>
-    <row r="38" spans="7:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="7:13" x14ac:dyDescent="0.3">
       <c r="G38" t="s">
         <v>15</v>
       </c>
@@ -1239,7 +1250,7 @@
         <v>5.4405339337378698E-2</v>
       </c>
     </row>
-    <row r="39" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G39" t="s">
         <v>15</v>
       </c>
@@ -1262,7 +1273,7 @@
         <v>7.4955341193283301E-2</v>
       </c>
     </row>
-    <row r="40" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G40" t="s">
         <v>15</v>
       </c>
@@ -1285,7 +1296,7 @@
         <v>0.70565235784035996</v>
       </c>
     </row>
-    <row r="41" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G41" t="s">
         <v>15</v>
       </c>
@@ -1308,7 +1319,7 @@
         <v>3.9433125328922597E-2</v>
       </c>
     </row>
-    <row r="42" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G42" t="s">
         <v>15</v>
       </c>
@@ -1331,12 +1342,12 @@
         <v>0.75576368876080602</v>
       </c>
     </row>
-    <row r="43" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="H43" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="H44" t="s">
         <v>16</v>
       </c>
@@ -1356,7 +1367,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G45" t="s">
         <v>16</v>
       </c>
@@ -1379,7 +1390,7 @@
         <v>0.76793786228705097</v>
       </c>
     </row>
-    <row r="46" spans="7:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="7:13" x14ac:dyDescent="0.3">
       <c r="G46" t="s">
         <v>16</v>
       </c>
@@ -1402,7 +1413,7 @@
         <v>5.4367369884870301E-2</v>
       </c>
     </row>
-    <row r="47" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G47" t="s">
         <v>16</v>
       </c>
@@ -1425,7 +1436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G48" t="s">
         <v>16</v>
       </c>
@@ -1448,7 +1459,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="49" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G49" t="s">
         <v>16</v>
       </c>
@@ -1471,7 +1482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G50" t="s">
         <v>16</v>
       </c>
@@ -1494,12 +1505,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="H51" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="H52" t="s">
         <v>17</v>
       </c>
@@ -1519,7 +1530,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G53" t="s">
         <v>17</v>
       </c>
@@ -1542,7 +1553,7 @@
         <v>0.76793786228705097</v>
       </c>
     </row>
-    <row r="54" spans="7:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="7:13" x14ac:dyDescent="0.3">
       <c r="G54" t="s">
         <v>17</v>
       </c>
@@ -1565,7 +1576,7 @@
         <v>5.4367369884870301E-2</v>
       </c>
     </row>
-    <row r="55" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G55" t="s">
         <v>17</v>
       </c>
@@ -1588,7 +1599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G56" t="s">
         <v>17</v>
       </c>
@@ -1611,7 +1622,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="57" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G57" t="s">
         <v>17</v>
       </c>
@@ -1634,7 +1645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G58" t="s">
         <v>17</v>
       </c>
@@ -1657,12 +1668,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="H59" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="H60" t="s">
         <v>18</v>
       </c>
@@ -1682,7 +1693,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G61" t="s">
         <v>18</v>
       </c>
@@ -1705,7 +1716,7 @@
         <v>0.770707290922934</v>
       </c>
     </row>
-    <row r="62" spans="7:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="7:13" x14ac:dyDescent="0.3">
       <c r="G62" t="s">
         <v>18</v>
       </c>
@@ -1728,7 +1739,7 @@
         <v>5.6233956008445503E-2</v>
       </c>
     </row>
-    <row r="63" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G63" t="s">
         <v>18</v>
       </c>
@@ -1751,7 +1762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G64" t="s">
         <v>18</v>
       </c>
@@ -1774,7 +1785,7 @@
         <v>0.49993933920170303</v>
       </c>
     </row>
-    <row r="65" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G65" t="s">
         <v>18</v>
       </c>
@@ -1797,7 +1808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G66" t="s">
         <v>18</v>
       </c>
@@ -1820,7 +1831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="H67" t="s">
         <v>2</v>
       </c>
@@ -1839,31 +1850,241 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5F33293-CDEC-4A94-AF6F-4699969CC4D9}">
+  <dimension ref="D3:I12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:I12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="32.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="E3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+    </row>
+    <row r="4" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="F4">
+        <v>0.2</v>
+      </c>
+      <c r="G4">
+        <v>0.3</v>
+      </c>
+      <c r="H4">
+        <v>0.4</v>
+      </c>
+      <c r="I4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="5">
+        <v>5.7689295126756503E-2</v>
+      </c>
+      <c r="F5" s="5">
+        <v>5.8772786410951697E-2</v>
+      </c>
+      <c r="G5" s="5">
+        <v>5.9296553380309702E-2</v>
+      </c>
+      <c r="H5" s="5">
+        <v>5.9507064414521603E-2</v>
+      </c>
+      <c r="I5" s="5">
+        <v>5.7933169700369401E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="5">
+        <v>5.7762066914832398E-2</v>
+      </c>
+      <c r="F6" s="5">
+        <v>5.8124018432318299E-2</v>
+      </c>
+      <c r="G6" s="5">
+        <v>5.8756027165059302E-2</v>
+      </c>
+      <c r="H6" s="5">
+        <v>5.9368922351429702E-2</v>
+      </c>
+      <c r="I6" s="5">
+        <v>5.9261662580175199E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="5">
+        <v>5.7733671547535802E-2</v>
+      </c>
+      <c r="F7" s="5">
+        <v>5.81077454763907E-2</v>
+      </c>
+      <c r="G7" s="5">
+        <v>6.0008233455203799E-2</v>
+      </c>
+      <c r="H7" s="5">
+        <v>5.8978727522389897E-2</v>
+      </c>
+      <c r="I7" s="5">
+        <v>5.8675491365870198E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="5">
+        <v>4.3545377864207903E-2</v>
+      </c>
+      <c r="F8" s="5">
+        <v>4.3540544353604202E-2</v>
+      </c>
+      <c r="G8" s="5">
+        <v>4.0530431470452502E-2</v>
+      </c>
+      <c r="H8" s="5">
+        <v>4.1215789071383298E-2</v>
+      </c>
+      <c r="I8" s="5">
+        <v>3.6736872561912902E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="5">
+        <v>5.7699364474209799E-2</v>
+      </c>
+      <c r="F9" s="5">
+        <v>5.9058682631689501E-2</v>
+      </c>
+      <c r="G9" s="5">
+        <v>5.7742473563534499E-2</v>
+      </c>
+      <c r="H9" s="5">
+        <v>5.7287875377566098E-2</v>
+      </c>
+      <c r="I9" s="5">
+        <v>5.4405339337378698E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="5">
+        <v>5.5481419280820399E-2</v>
+      </c>
+      <c r="F10" s="5">
+        <v>5.6058063508783999E-2</v>
+      </c>
+      <c r="G10" s="5">
+        <v>5.4659268433653603E-2</v>
+      </c>
+      <c r="H10" s="5">
+        <v>5.8427183066308598E-2</v>
+      </c>
+      <c r="I10" s="5">
+        <v>5.4367369884870301E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="5">
+        <v>5.69316136297289E-2</v>
+      </c>
+      <c r="F11" s="5">
+        <v>5.78541594050897E-2</v>
+      </c>
+      <c r="G11" s="5">
+        <v>5.6997832360600499E-2</v>
+      </c>
+      <c r="H11" s="5">
+        <v>5.4977864672537E-2</v>
+      </c>
+      <c r="I11" s="5">
+        <v>5.4367369884870301E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="5">
+        <v>5.57438493220462E-2</v>
+      </c>
+      <c r="F12" s="5">
+        <v>5.4951425953852301E-2</v>
+      </c>
+      <c r="G12" s="5">
+        <v>5.4953792376000503E-2</v>
+      </c>
+      <c r="H12" s="5">
+        <v>5.75131836484815E-2</v>
+      </c>
+      <c r="I12" s="5">
+        <v>5.6233956008445503E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E3:I3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82F85408-8434-4342-B878-6856944D828F}">
   <sheetPr filterMode="1"/>
   <dimension ref="G1:M66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="8" max="8" width="62.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="62.5546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="7:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="7:13" x14ac:dyDescent="0.3">
       <c r="H1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="7:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="7:13" x14ac:dyDescent="0.3">
       <c r="H2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="7:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="7:13" x14ac:dyDescent="0.3">
       <c r="H3" s="4" t="s">
         <v>3</v>
       </c>
@@ -1883,7 +2104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="H4" t="s">
         <v>4</v>
       </c>
@@ -1903,7 +2124,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G5" t="s">
         <v>4</v>
       </c>
@@ -1926,7 +2147,7 @@
         <v>0.76458743606287705</v>
       </c>
     </row>
-    <row r="6" spans="7:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="7:13" x14ac:dyDescent="0.3">
       <c r="G6" t="s">
         <v>4</v>
       </c>
@@ -1949,7 +2170,7 @@
         <v>5.6010153532493098E-2</v>
       </c>
     </row>
-    <row r="7" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G7" t="s">
         <v>4</v>
       </c>
@@ -1972,7 +2193,7 @@
         <v>7.5356257744733507E-2</v>
       </c>
     </row>
-    <row r="8" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G8" t="s">
         <v>4</v>
       </c>
@@ -1995,7 +2216,7 @@
         <v>0.69236162160862302</v>
       </c>
     </row>
-    <row r="9" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G9" t="s">
         <v>4</v>
       </c>
@@ -2018,7 +2239,7 @@
         <v>3.9818300867572397E-2</v>
       </c>
     </row>
-    <row r="10" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G10" t="s">
         <v>4</v>
       </c>
@@ -2041,12 +2262,12 @@
         <v>0.70100864553314102</v>
       </c>
     </row>
-    <row r="11" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="H11" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="H12" t="s">
         <v>12</v>
       </c>
@@ -2066,7 +2287,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G13" t="s">
         <v>12</v>
       </c>
@@ -2089,7 +2310,7 @@
         <v>0.76779373704742304</v>
       </c>
     </row>
-    <row r="14" spans="7:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="7:13" x14ac:dyDescent="0.3">
       <c r="G14" t="s">
         <v>12</v>
       </c>
@@ -2112,7 +2333,7 @@
         <v>5.6598844197761497E-2</v>
       </c>
     </row>
-    <row r="15" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G15" t="s">
         <v>12</v>
       </c>
@@ -2135,7 +2356,7 @@
         <v>8.2526239920717101E-2</v>
       </c>
     </row>
-    <row r="16" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G16" t="s">
         <v>12</v>
       </c>
@@ -2158,7 +2379,7 @@
         <v>0.695877116878304</v>
       </c>
     </row>
-    <row r="17" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G17" t="s">
         <v>12</v>
       </c>
@@ -2181,7 +2402,7 @@
         <v>4.4015184277545499E-2</v>
       </c>
     </row>
-    <row r="18" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G18" t="s">
         <v>12</v>
       </c>
@@ -2204,12 +2425,12 @@
         <v>0.65994236311239196</v>
       </c>
     </row>
-    <row r="19" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="H19" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="H20" t="s">
         <v>13</v>
       </c>
@@ -2229,7 +2450,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G21" t="s">
         <v>13</v>
       </c>
@@ -2252,7 +2473,7 @@
         <v>0.76630102106322395</v>
       </c>
     </row>
-    <row r="22" spans="7:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="7:13" x14ac:dyDescent="0.3">
       <c r="G22" t="s">
         <v>13</v>
       </c>
@@ -2275,7 +2496,7 @@
         <v>5.6883910922848502E-2</v>
       </c>
     </row>
-    <row r="23" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G23" t="s">
         <v>13</v>
       </c>
@@ -2298,7 +2519,7 @@
         <v>7.3973607038123099E-2</v>
       </c>
     </row>
-    <row r="24" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G24" t="s">
         <v>13</v>
       </c>
@@ -2321,7 +2542,7 @@
         <v>0.69575899536705299</v>
       </c>
     </row>
-    <row r="25" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G25" t="s">
         <v>13</v>
       </c>
@@ -2344,7 +2565,7 @@
         <v>3.8969565889077698E-2</v>
       </c>
     </row>
-    <row r="26" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G26" t="s">
         <v>13</v>
       </c>
@@ -2367,12 +2588,12 @@
         <v>0.72694524495677204</v>
       </c>
     </row>
-    <row r="27" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="H27" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="H28" t="s">
         <v>14</v>
       </c>
@@ -2392,7 +2613,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G29" t="s">
         <v>14</v>
       </c>
@@ -2415,7 +2636,7 @@
         <v>0.70593220263262801</v>
       </c>
     </row>
-    <row r="30" spans="7:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="7:13" x14ac:dyDescent="0.3">
       <c r="G30" t="s">
         <v>14</v>
       </c>
@@ -2438,7 +2659,7 @@
         <v>4.1439442119660802E-2</v>
       </c>
     </row>
-    <row r="31" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G31" t="s">
         <v>14</v>
       </c>
@@ -2461,7 +2682,7 @@
         <v>4.5172623955831201E-2</v>
       </c>
     </row>
-    <row r="32" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G32" t="s">
         <v>14</v>
       </c>
@@ -2484,7 +2705,7 @@
         <v>0.59573565659593797</v>
       </c>
     </row>
-    <row r="33" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G33" t="s">
         <v>14</v>
       </c>
@@ -2507,7 +2728,7 @@
         <v>2.3162616272657002E-2</v>
       </c>
     </row>
-    <row r="34" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G34" t="s">
         <v>14</v>
       </c>
@@ -2530,12 +2751,12 @@
         <v>0.90778097982708905</v>
       </c>
     </row>
-    <row r="35" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="H35" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="H36" t="s">
         <v>15</v>
       </c>
@@ -2555,7 +2776,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G37" t="s">
         <v>15</v>
       </c>
@@ -2578,7 +2799,7 @@
         <v>0.76669148003451604</v>
       </c>
     </row>
-    <row r="38" spans="7:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="7:13" x14ac:dyDescent="0.3">
       <c r="G38" t="s">
         <v>15</v>
       </c>
@@ -2601,7 +2822,7 @@
         <v>5.7226069278240303E-2</v>
       </c>
     </row>
-    <row r="39" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G39" t="s">
         <v>15</v>
       </c>
@@ -2624,7 +2845,7 @@
         <v>7.5381034612208103E-2</v>
       </c>
     </row>
-    <row r="40" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G40" t="s">
         <v>15</v>
       </c>
@@ -2647,7 +2868,7 @@
         <v>0.698251279130925</v>
       </c>
     </row>
-    <row r="41" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G41" t="s">
         <v>15</v>
       </c>
@@ -2670,7 +2891,7 @@
         <v>3.9762376237623701E-2</v>
       </c>
     </row>
-    <row r="42" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G42" t="s">
         <v>15</v>
       </c>
@@ -2693,12 +2914,12 @@
         <v>0.72334293948126804</v>
       </c>
     </row>
-    <row r="43" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="H43" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="H44" t="s">
         <v>16</v>
       </c>
@@ -2718,7 +2939,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G45" t="s">
         <v>16</v>
       </c>
@@ -2741,7 +2962,7 @@
         <v>0.76347383550011305</v>
       </c>
     </row>
-    <row r="46" spans="7:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="7:13" x14ac:dyDescent="0.3">
       <c r="G46" t="s">
         <v>16</v>
       </c>
@@ -2764,7 +2985,7 @@
         <v>5.4453197601791001E-2</v>
       </c>
     </row>
-    <row r="47" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G47" t="s">
         <v>16</v>
       </c>
@@ -2787,7 +3008,7 @@
         <v>0.107883817427385</v>
       </c>
     </row>
-    <row r="48" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G48" t="s">
         <v>16</v>
       </c>
@@ -2810,7 +3031,7 @@
         <v>0.641498032690479</v>
       </c>
     </row>
-    <row r="49" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G49" t="s">
         <v>16</v>
       </c>
@@ -2833,7 +3054,7 @@
         <v>6.2514311884588905E-2</v>
       </c>
     </row>
-    <row r="50" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G50" t="s">
         <v>16</v>
       </c>
@@ -2856,12 +3077,12 @@
         <v>0.39337175792507201</v>
       </c>
     </row>
-    <row r="51" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="H51" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="H52" t="s">
         <v>17</v>
       </c>
@@ -2881,7 +3102,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G53" t="s">
         <v>17</v>
       </c>
@@ -2904,7 +3125,7 @@
         <v>0.76347383550011305</v>
       </c>
     </row>
-    <row r="54" spans="7:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="7:13" x14ac:dyDescent="0.3">
       <c r="G54" t="s">
         <v>17</v>
       </c>
@@ -2927,7 +3148,7 @@
         <v>5.4453197601791001E-2</v>
       </c>
     </row>
-    <row r="55" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G55" t="s">
         <v>17</v>
       </c>
@@ -2950,7 +3171,7 @@
         <v>0.107883817427385</v>
       </c>
     </row>
-    <row r="56" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G56" t="s">
         <v>17</v>
       </c>
@@ -2973,7 +3194,7 @@
         <v>0.641498032690479</v>
       </c>
     </row>
-    <row r="57" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G57" t="s">
         <v>17</v>
       </c>
@@ -2996,7 +3217,7 @@
         <v>6.2514311884588905E-2</v>
       </c>
     </row>
-    <row r="58" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G58" t="s">
         <v>17</v>
       </c>
@@ -3019,12 +3240,12 @@
         <v>0.39337175792507201</v>
       </c>
     </row>
-    <row r="59" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="H59" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="H60" t="s">
         <v>18</v>
       </c>
@@ -3044,7 +3265,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G61" t="s">
         <v>18</v>
       </c>
@@ -3067,7 +3288,7 @@
         <v>0.76573517410659098</v>
       </c>
     </row>
-    <row r="62" spans="7:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="7:13" x14ac:dyDescent="0.3">
       <c r="G62" t="s">
         <v>18</v>
       </c>
@@ -3090,7 +3311,7 @@
         <v>5.5077222956431998E-2</v>
       </c>
     </row>
-    <row r="63" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G63" t="s">
         <v>18</v>
       </c>
@@ -3113,7 +3334,7 @@
         <v>0.10229103902473199</v>
       </c>
     </row>
-    <row r="64" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G64" t="s">
         <v>18</v>
       </c>
@@ -3136,7 +3357,7 @@
         <v>0.68104252156857503</v>
       </c>
     </row>
-    <row r="65" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G65" t="s">
         <v>18</v>
       </c>
@@ -3159,7 +3380,7 @@
         <v>5.6655025223127597E-2</v>
       </c>
     </row>
-    <row r="66" spans="7:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="7:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="G66" t="s">
         <v>18</v>
       </c>

</xml_diff>